<commit_message>
Implementing Ziegler Nichols in progress
</commit_message>
<xml_diff>
--- a/20230208_coolingflow_biotemp.xlsx
+++ b/20230208_coolingflow_biotemp.xlsx
@@ -13,7 +13,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Kp</t>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>Td</t>
+  </si>
   <si>
     <t>Step</t>
   </si>
@@ -121,24 +133,24 @@
   <dimension ref="A1:D39"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="true"/>
-    <col min="2" max="2" width="15.1875" customWidth="true"/>
-    <col min="3" max="3" width="11.60546875" customWidth="true"/>
-    <col min="4" max="4" width="14.60546875" customWidth="true"/>
+    <col min="1" max="1" width="5.140625" customWidth="true"/>
+    <col min="2" max="2" width="15.42578125" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="14.7109375" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
@@ -146,13 +158,13 @@
         <v>-100</v>
       </c>
       <c r="B2" s="0">
-        <v>-0.0017744319248317098</v>
+        <v>-0.0017744322561683745</v>
       </c>
       <c r="C2" s="0">
-        <v>6.3865382477674757</v>
+        <v>6.3915631747415773</v>
       </c>
       <c r="D2" s="0">
-        <v>0.002216261611124537</v>
+        <v>0.0022006376404988259</v>
       </c>
     </row>
     <row r="3">
@@ -160,13 +172,13 @@
         <v>-95</v>
       </c>
       <c r="B3" s="0">
-        <v>-0.0017546484781527439</v>
+        <v>-0.0017546484768851357</v>
       </c>
       <c r="C3" s="0">
-        <v>6.3897016238256867</v>
+        <v>6.3896312101279307</v>
       </c>
       <c r="D3" s="0">
-        <v>0.0021673159901922645</v>
+        <v>0.0021829201454863778</v>
       </c>
     </row>
     <row r="4">
@@ -174,13 +186,13 @@
         <v>-90</v>
       </c>
       <c r="B4" s="0">
-        <v>-0.0017353000872278399</v>
+        <v>-0.0017353000856968571</v>
       </c>
       <c r="C4" s="0">
-        <v>6.3887108534058825</v>
+        <v>6.3914656056209651</v>
       </c>
       <c r="D4" s="0">
-        <v>0.0021437129429955348</v>
+        <v>0.0021512166887305284</v>
       </c>
     </row>
     <row r="5">
@@ -188,13 +200,13 @@
         <v>-85</v>
       </c>
       <c r="B5" s="0">
-        <v>-0.0017163729190665955</v>
+        <v>-0.0017163729211930826</v>
       </c>
       <c r="C5" s="0">
-        <v>6.3896046761774983</v>
+        <v>6.3930346850799538</v>
       </c>
       <c r="D5" s="0">
-        <v>0.0021080213479649501</v>
+        <v>0.0020937014231776629</v>
       </c>
     </row>
     <row r="6">
@@ -202,13 +214,13 @@
         <v>-80</v>
       </c>
       <c r="B6" s="0">
-        <v>-0.0016978534190014826</v>
+        <v>-0.0016978534186095295</v>
       </c>
       <c r="C6" s="0">
-        <v>6.3892053792783372</v>
+        <v>6.3943523987966842</v>
       </c>
       <c r="D6" s="0">
-        <v>0.0020991822343034983</v>
+        <v>0.0020634277604472118</v>
       </c>
     </row>
     <row r="7">
@@ -216,13 +228,13 @@
         <v>-75</v>
       </c>
       <c r="B7" s="0">
-        <v>-0.001679728398596012</v>
+        <v>-0.001679728597720119</v>
       </c>
       <c r="C7" s="0">
-        <v>6.3887321065661808</v>
+        <v>6.3932594462000907</v>
       </c>
       <c r="D7" s="0">
-        <v>0.002073896708338907</v>
+        <v>0.0020445930451842287</v>
       </c>
     </row>
     <row r="8">
@@ -230,13 +242,13 @@
         <v>-70</v>
       </c>
       <c r="B8" s="0">
-        <v>-0.0016619860343813084</v>
+        <v>-0.0016619860296646749</v>
       </c>
       <c r="C8" s="0">
-        <v>6.3885089010820479</v>
+        <v>6.3923727045312262</v>
       </c>
       <c r="D8" s="0">
-        <v>0.0020479341375789772</v>
+        <v>0.0020377660228518835</v>
       </c>
     </row>
     <row r="9">
@@ -244,13 +256,13 @@
         <v>-65</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.0016446138286250053</v>
+        <v>-0.0016446136777998478</v>
       </c>
       <c r="C9" s="0">
-        <v>6.3885420921890272</v>
+        <v>6.3910813820477301</v>
       </c>
       <c r="D9" s="0">
-        <v>0.0020210727203107126</v>
+        <v>0.0020136352700887983</v>
       </c>
     </row>
     <row r="10">
@@ -258,13 +270,13 @@
         <v>-60</v>
       </c>
       <c r="B10" s="0">
-        <v>-0.0016276005829646205</v>
+        <v>-0.0016276005828804211</v>
       </c>
       <c r="C10" s="0">
-        <v>6.39637063213695</v>
+        <v>6.3920518110119815</v>
       </c>
       <c r="D10" s="0">
-        <v>0.0019644960091227404</v>
+        <v>0.0019271221562462415</v>
       </c>
     </row>
     <row r="11">
@@ -272,13 +284,13 @@
         <v>-55</v>
       </c>
       <c r="B11" s="0">
-        <v>-0.0016109353828401719</v>
+        <v>-0.0016109353851111957</v>
       </c>
       <c r="C11" s="0">
-        <v>6.3968599490702047</v>
+        <v>6.3940722556190792</v>
       </c>
       <c r="D11" s="0">
-        <v>0.0019411386889203186</v>
+        <v>0.0018932943742981934</v>
       </c>
     </row>
     <row r="12">
@@ -286,13 +298,13 @@
         <v>-50</v>
       </c>
       <c r="B12" s="0">
-        <v>-0.0015946077910836466</v>
+        <v>-0.0015946077843322114</v>
       </c>
       <c r="C12" s="0">
-        <v>6.3916180220699914</v>
+        <v>6.3958964686983393</v>
       </c>
       <c r="D12" s="0">
-        <v>0.0018608959392452107</v>
+        <v>0.0018424001174537352</v>
       </c>
     </row>
     <row r="13">
@@ -300,13 +312,13 @@
         <v>-45</v>
       </c>
       <c r="B13" s="0">
-        <v>-0.0015786078127695033</v>
+        <v>-0.0015786078173101873</v>
       </c>
       <c r="C13" s="0">
-        <v>6.3939385471219907</v>
+        <v>6.3953097510055272</v>
       </c>
       <c r="D13" s="0">
-        <v>0.0018232698962492577</v>
+        <v>0.0018266859144659975</v>
       </c>
     </row>
     <row r="14">
@@ -314,13 +326,13 @@
         <v>-40</v>
       </c>
       <c r="B14" s="0">
-        <v>-0.0015629259234689386</v>
+        <v>-0.0015629259432118126</v>
       </c>
       <c r="C14" s="0">
-        <v>6.3932193508302362</v>
+        <v>6.3926325367935419</v>
       </c>
       <c r="D14" s="0">
-        <v>0.0017761031539862415</v>
+        <v>0.0018006456635362156</v>
       </c>
     </row>
     <row r="15">
@@ -328,13 +340,13 @@
         <v>-35</v>
       </c>
       <c r="B15" s="0">
-        <v>-0.0015475531601701676</v>
+        <v>-0.001547553160627351</v>
       </c>
       <c r="C15" s="0">
-        <v>6.3920379414676631</v>
+        <v>6.3931464228083428</v>
       </c>
       <c r="D15" s="0">
-        <v>0.0017457868199244331</v>
+        <v>0.0017636869731063598</v>
       </c>
     </row>
     <row r="16">
@@ -342,13 +354,13 @@
         <v>-30</v>
       </c>
       <c r="B16" s="0">
-        <v>-0.0015324810004522977</v>
+        <v>-0.0015324809936390219</v>
       </c>
       <c r="C16" s="0">
-        <v>6.395049705006528</v>
+        <v>6.3944579724108905</v>
       </c>
       <c r="D16" s="0">
-        <v>0.0016959161071383733</v>
+        <v>0.0017181683361684463</v>
       </c>
     </row>
     <row r="17">
@@ -356,13 +368,13 @@
         <v>-25</v>
       </c>
       <c r="B17" s="0">
-        <v>-0.0015177017665828885</v>
+        <v>-0.0015177017718116304</v>
       </c>
       <c r="C17" s="0">
-        <v>6.3988155302217251</v>
+        <v>6.3961071124483908</v>
       </c>
       <c r="D17" s="0">
-        <v>0.0016312621752376799</v>
+        <v>0.0016607763675153819</v>
       </c>
     </row>
     <row r="18">
@@ -370,13 +382,13 @@
         <v>-20</v>
       </c>
       <c r="B18" s="0">
-        <v>-0.0015032090298253919</v>
+        <v>-0.0015032090467771652</v>
       </c>
       <c r="C18" s="0">
-        <v>6.3932677908441065</v>
+        <v>6.3932678629192594</v>
       </c>
       <c r="D18" s="0">
-        <v>0.0015903474231890868</v>
+        <v>0.0015903474187837219</v>
       </c>
     </row>
     <row r="19">
@@ -384,13 +396,13 @@
         <v>-15</v>
       </c>
       <c r="B19" s="0">
-        <v>-0.0014889991507935462</v>
+        <v>-0.0014889991678188608</v>
       </c>
       <c r="C19" s="0">
-        <v>6.3959942991729974</v>
+        <v>6.3959943724668165</v>
       </c>
       <c r="D19" s="0">
-        <v>0.001477648824533162</v>
+        <v>0.0014776488192751458</v>
       </c>
     </row>
     <row r="20">
@@ -398,13 +410,13 @@
         <v>-10</v>
       </c>
       <c r="B20" s="0">
-        <v>-0.0014750774984257475</v>
+        <v>-0.0014750774984261029</v>
       </c>
       <c r="C20" s="0">
-        <v>6.3969058415449354</v>
+        <v>6.3969058407871842</v>
       </c>
       <c r="D20" s="0">
-        <v>0.0012767646312568104</v>
+        <v>0.0012767646326494742</v>
       </c>
     </row>
     <row r="21">
@@ -412,13 +424,13 @@
         <v>10</v>
       </c>
       <c r="B21" s="0">
-        <v>-0.0014214766946214041</v>
+        <v>-0.0014214766946217595</v>
       </c>
       <c r="C21" s="0">
-        <v>6.3981792300243967</v>
+        <v>6.3981792300865266</v>
       </c>
       <c r="D21" s="0">
-        <v>0.0023622786886505764</v>
+        <v>0.002362278685467345</v>
       </c>
     </row>
     <row r="22">
@@ -426,13 +438,13 @@
         <v>15</v>
       </c>
       <c r="B22" s="0">
-        <v>-0.0014087815947263493</v>
+        <v>-0.0014087815947261126</v>
       </c>
       <c r="C22" s="0">
-        <v>6.3989534862864446</v>
+        <v>6.3989534863458744</v>
       </c>
       <c r="D22" s="0">
-        <v>0.00216005806524322</v>
+        <v>0.0021600580631115918</v>
       </c>
     </row>
     <row r="23">
@@ -440,13 +452,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="0">
-        <v>-0.0013962907602126152</v>
+        <v>-0.0013962906350025507</v>
       </c>
       <c r="C23" s="0">
-        <v>6.4040496861732663</v>
+        <v>6.4016196452336089</v>
       </c>
       <c r="D23" s="0">
-        <v>0.0020421491340698594</v>
+        <v>0.0020444594816808603</v>
       </c>
     </row>
     <row r="24">
@@ -454,13 +466,13 @@
         <v>25</v>
       </c>
       <c r="B24" s="0">
-        <v>-0.0013840109244016218</v>
+        <v>-0.001384010933844877</v>
       </c>
       <c r="C24" s="0">
-        <v>6.4026663807042326</v>
+        <v>6.4003559520797921</v>
       </c>
       <c r="D24" s="0">
-        <v>0.0019828052208197278</v>
+        <v>0.0019804153848212991</v>
       </c>
     </row>
     <row r="25">
@@ -468,13 +480,13 @@
         <v>30</v>
       </c>
       <c r="B25" s="0">
-        <v>-0.0013719411915964486</v>
+        <v>-0.0013719410729131928</v>
       </c>
       <c r="C25" s="0">
-        <v>6.4018258002711264</v>
+        <v>6.3995069299533327</v>
       </c>
       <c r="D25" s="0">
-        <v>0.0019393833257481674</v>
+        <v>0.0019333505311180943</v>
       </c>
     </row>
     <row r="26">
@@ -482,13 +494,13 @@
         <v>35</v>
       </c>
       <c r="B26" s="0">
-        <v>-0.0013600775065987542</v>
+        <v>-0.0013600773778733809</v>
       </c>
       <c r="C26" s="0">
-        <v>6.4013342386952559</v>
+        <v>6.3994466339350708</v>
       </c>
       <c r="D26" s="0">
-        <v>0.0019050551705959151</v>
+        <v>0.0018947552757424546</v>
       </c>
     </row>
     <row r="27">
@@ -496,13 +508,13 @@
         <v>40</v>
       </c>
       <c r="B27" s="0">
-        <v>-0.0013484154479895595</v>
+        <v>-0.0013484155632164986</v>
       </c>
       <c r="C27" s="0">
-        <v>6.3998898038928758</v>
+        <v>6.4008812747760828</v>
       </c>
       <c r="D27" s="0">
-        <v>0.0018533634998050275</v>
+        <v>0.0018593401195232673</v>
       </c>
     </row>
     <row r="28">
@@ -510,13 +522,13 @@
         <v>45</v>
       </c>
       <c r="B28" s="0">
-        <v>-0.0013369505976099402</v>
+        <v>-0.0013369506076670412</v>
       </c>
       <c r="C28" s="0">
-        <v>6.3990362278300097</v>
+        <v>6.4022239179289215</v>
       </c>
       <c r="D28" s="0">
-        <v>0.001827744860833036</v>
+        <v>0.0018288270466371159</v>
       </c>
     </row>
     <row r="29">
@@ -524,13 +536,13 @@
         <v>50</v>
       </c>
       <c r="B29" s="0">
-        <v>-0.0013256781752628655</v>
+        <v>-0.001325678177805969</v>
       </c>
       <c r="C29" s="0">
-        <v>6.3986466866977025</v>
+        <v>6.4034676017519701</v>
       </c>
       <c r="D29" s="0">
-        <v>0.001803728258494175</v>
+        <v>0.0018018500165908335</v>
       </c>
     </row>
     <row r="30">
@@ -538,13 +550,13 @@
         <v>55</v>
       </c>
       <c r="B30" s="0">
-        <v>-0.0013145935165110503</v>
+        <v>-0.0013145935168683888</v>
       </c>
       <c r="C30" s="0">
-        <v>6.3997983820537456</v>
+        <v>6.3885393967715061</v>
       </c>
       <c r="D30" s="0">
-        <v>0.0017786615983936827</v>
+        <v>0.0017761489942529352</v>
       </c>
     </row>
     <row r="31">
@@ -552,13 +564,13 @@
         <v>60</v>
       </c>
       <c r="B31" s="0">
-        <v>-0.0013036921021728413</v>
+        <v>-0.0013036920888413424</v>
       </c>
       <c r="C31" s="0">
-        <v>6.4009135910504256</v>
+        <v>6.39055870128945</v>
       </c>
       <c r="D31" s="0">
-        <v>0.0017551562582411862</v>
+        <v>0.0017524799592081308</v>
       </c>
     </row>
     <row r="32">
@@ -566,13 +578,13 @@
         <v>65</v>
       </c>
       <c r="B32" s="0">
-        <v>-0.0012929694788493971</v>
+        <v>-0.0012929694873630654</v>
       </c>
       <c r="C32" s="0">
-        <v>6.4020858534876766</v>
+        <v>6.3903036662872807</v>
       </c>
       <c r="D32" s="0">
-        <v>0.0017331566710367952</v>
+        <v>0.0017329900138918219</v>
       </c>
     </row>
     <row r="33">
@@ -580,13 +592,13 @@
         <v>70</v>
       </c>
       <c r="B33" s="0">
-        <v>-0.001282421375330957</v>
+        <v>-0.0012824213769623632</v>
       </c>
       <c r="C33" s="0">
-        <v>6.3987538174073393</v>
+        <v>6.3879912256835496</v>
       </c>
       <c r="D33" s="0">
-        <v>0.0017225270892140543</v>
+        <v>0.0017119740862767685</v>
       </c>
     </row>
     <row r="34">
@@ -594,13 +606,13 @@
         <v>75</v>
       </c>
       <c r="B34" s="0">
-        <v>-0.0012720435811526443</v>
+        <v>-0.0012720435706664072</v>
       </c>
       <c r="C34" s="0">
-        <v>6.39922577992985</v>
+        <v>6.3878456028654682</v>
       </c>
       <c r="D34" s="0">
-        <v>0.0017041614766526436</v>
+        <v>0.0016950773276107611</v>
       </c>
     </row>
     <row r="35">
@@ -608,13 +620,13 @@
         <v>80</v>
       </c>
       <c r="B35" s="0">
-        <v>-0.0012618320470878519</v>
+        <v>-0.0012618320398253946</v>
       </c>
       <c r="C35" s="0">
-        <v>6.3983627900534259</v>
+        <v>6.3890621817031956</v>
       </c>
       <c r="D35" s="0">
-        <v>0.0016740422459804449</v>
+        <v>0.0016574021665860528</v>
       </c>
     </row>
     <row r="36">
@@ -622,13 +634,13 @@
         <v>85</v>
       </c>
       <c r="B36" s="0">
-        <v>-0.0012517828315429574</v>
+        <v>-0.0012517828267786012</v>
       </c>
       <c r="C36" s="0">
-        <v>6.398421718025503</v>
+        <v>6.3888896334588026</v>
       </c>
       <c r="D36" s="0">
-        <v>0.0016572636820058051</v>
+        <v>0.0016407726380975873</v>
       </c>
     </row>
     <row r="37">
@@ -636,13 +648,13 @@
         <v>90</v>
       </c>
       <c r="B37" s="0">
-        <v>-0.0012418921135177482</v>
+        <v>-0.0012418921135176693</v>
       </c>
       <c r="C37" s="0">
-        <v>6.3947955742899296</v>
+        <v>6.3947955743285263</v>
       </c>
       <c r="D37" s="0">
-        <v>0.0016327333170522706</v>
+        <v>0.0016327333180754522</v>
       </c>
     </row>
     <row r="38">
@@ -650,13 +662,13 @@
         <v>95</v>
       </c>
       <c r="B38" s="0">
-        <v>-0.0012321561755304943</v>
+        <v>-0.0012321561752906675</v>
       </c>
       <c r="C38" s="0">
-        <v>6.3944011603708191</v>
+        <v>6.3944011591110268</v>
       </c>
       <c r="D38" s="0">
-        <v>0.0016194677078260611</v>
+        <v>0.001619467708422917</v>
       </c>
     </row>
     <row r="39">
@@ -664,13 +676,13 @@
         <v>100</v>
       </c>
       <c r="B39" s="0">
-        <v>-0.0012225714742685411</v>
+        <v>-0.0012225714740245407</v>
       </c>
       <c r="C39" s="0">
-        <v>6.4003603057966245</v>
+        <v>6.4003603043488795</v>
       </c>
       <c r="D39" s="0">
-        <v>0.0015991194521518537</v>
+        <v>0.0015991194523223839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>